<commit_message>
added back fastq files that were found in LTS but had no metadata files
</commit_message>
<xml_diff>
--- a/library/library_3275.xlsx
+++ b/library/library_3275.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29FF94F-974D-684F-BEEB-676E12260989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7356D685-8FA3-C447-A12C-8737E6C14C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14080" yWindow="460" windowWidth="16380" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="26720" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="41">
   <si>
     <t>s2cDNADate</t>
   </si>
@@ -528,15 +528,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1424,6 +1430,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36">
+        <v>36</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37">
+        <v>37</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>